<commit_message>
Añadido mejoría absoluta y relativa
</commit_message>
<xml_diff>
--- a/Generador_informe/Demo_All_VIM_Uni_AlejandroTFG.xlsx
+++ b/Generador_informe/Demo_All_VIM_Uni_AlejandroTFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/tfg/Generador_informe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF52C965-F2EF-064D-A4FE-0AC9AA457686}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D855B0-A2EF-2F42-828C-98BAF85FB97F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -595,7 +595,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Combinar las bbdd de pacientes en un único archivo
</commit_message>
<xml_diff>
--- a/Generador_informe/Demo_All_VIM_Uni_AlejandroTFG.xlsx
+++ b/Generador_informe/Demo_All_VIM_Uni_AlejandroTFG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/tfg/Generador_informe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D855B0-A2EF-2F42-828C-98BAF85FB97F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44CE1BA-5FB8-5F41-8012-23888242EFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="32420" windowHeight="20500" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demography_VIM" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
   <si>
     <t>Diag</t>
-  </si>
-  <si>
-    <t>ID_CT</t>
   </si>
   <si>
     <t>Gender</t>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Mejoria_Rel_HT</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,63 +623,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3">
         <v>3</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="3" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="4" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="5" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <v>6</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="6" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3">
         <v>8</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="7" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>12</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="8" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3">
         <v>13</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="9" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>14</v>
@@ -5079,7 +5079,7 @@
     </row>
     <row r="10" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3">
         <v>15</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="11" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3">
         <v>19</v>
@@ -7153,7 +7153,7 @@
     </row>
     <row r="12" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3">
         <v>23</v>
@@ -8190,7 +8190,7 @@
     </row>
     <row r="13" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3">
         <v>26</v>
@@ -9227,7 +9227,7 @@
     </row>
     <row r="14" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3">
         <v>30</v>
@@ -10264,7 +10264,7 @@
     </row>
     <row r="15" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3">
         <v>31</v>
@@ -10327,7 +10327,7 @@
     </row>
     <row r="16" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>49</v>
@@ -11364,7 +11364,7 @@
     </row>
     <row r="17" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
         <v>53</v>
@@ -12401,7 +12401,7 @@
     </row>
     <row r="18" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3">
         <v>63</v>
@@ -13438,7 +13438,7 @@
     </row>
     <row r="19" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3">
         <v>69</v>
@@ -14475,7 +14475,7 @@
     </row>
     <row r="20" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3">
         <v>75</v>
@@ -15512,7 +15512,7 @@
     </row>
     <row r="21" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3">
         <v>76</v>
@@ -16549,7 +16549,7 @@
     </row>
     <row r="22" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="3">
         <v>85</v>
@@ -17586,7 +17586,7 @@
     </row>
     <row r="23" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="3">
         <v>87</v>
@@ -18623,7 +18623,7 @@
     </row>
     <row r="24" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="3">
         <v>89</v>
@@ -19656,7 +19656,7 @@
     </row>
     <row r="25" spans="1:995" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="8">
         <v>91</v>
@@ -20693,7 +20693,7 @@
     </row>
     <row r="26" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="3">
         <v>95</v>
@@ -20756,7 +20756,7 @@
     </row>
     <row r="27" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="3">
         <v>99</v>
@@ -20819,7 +20819,7 @@
     </row>
     <row r="28" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3">
         <v>101</v>
@@ -20882,7 +20882,7 @@
     </row>
     <row r="29" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3">
         <v>102</v>
@@ -20941,7 +20941,7 @@
     </row>
     <row r="30" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3">
         <v>108</v>
@@ -21004,7 +21004,7 @@
     </row>
     <row r="31" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="3">
         <v>109</v>
@@ -21063,7 +21063,7 @@
     </row>
     <row r="32" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="3">
         <v>111</v>
@@ -22100,7 +22100,7 @@
     </row>
     <row r="33" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="3">
         <v>116</v>
@@ -22163,7 +22163,7 @@
     </row>
     <row r="34" spans="1:995" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="10">
         <v>121</v>
@@ -22226,7 +22226,7 @@
     </row>
     <row r="35" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="3">
         <v>131</v>
@@ -22289,7 +22289,7 @@
     </row>
     <row r="36" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="2">
         <v>133</v>
@@ -22352,7 +22352,7 @@
     </row>
     <row r="37" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="3">
         <v>134</v>
@@ -22411,7 +22411,7 @@
     </row>
     <row r="38" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="2">
         <v>141</v>
@@ -23448,7 +23448,7 @@
     </row>
     <row r="39" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" s="2">
         <v>142</v>
@@ -24485,7 +24485,7 @@
     </row>
     <row r="40" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" s="2">
         <v>143</v>
@@ -25522,7 +25522,7 @@
     </row>
     <row r="41" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="2">
         <v>145</v>
@@ -26559,7 +26559,7 @@
     </row>
     <row r="42" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" s="2">
         <v>147</v>
@@ -27592,7 +27592,7 @@
     </row>
     <row r="43" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="2">
         <v>155</v>
@@ -28625,7 +28625,7 @@
     </row>
     <row r="44" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" s="3">
         <v>156</v>
@@ -28684,7 +28684,7 @@
     </row>
     <row r="45" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="2">
         <v>157</v>
@@ -28743,7 +28743,7 @@
     </row>
     <row r="46" spans="1:995" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B46" s="2">
         <v>162</v>
@@ -28802,7 +28802,7 @@
     </row>
     <row r="47" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="2">
         <v>171</v>
@@ -28861,7 +28861,7 @@
     </row>
     <row r="48" spans="1:995" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" s="2">
         <v>174</v>
@@ -28920,7 +28920,7 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B49" s="2">
         <v>176</v>
@@ -28979,7 +28979,7 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B50" s="2">
         <v>177</v>
@@ -29038,7 +29038,7 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B51" s="2">
         <v>183</v>
@@ -29097,7 +29097,7 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" s="2">
         <v>188</v>
@@ -29152,7 +29152,7 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B53" s="3">
         <v>901</v>
@@ -29215,7 +29215,7 @@
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54" s="3">
         <v>904</v>
@@ -29278,7 +29278,7 @@
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" s="3">
         <v>907</v>

</xml_diff>